<commit_message>
Palabras largas -> 10 chars
</commit_message>
<xml_diff>
--- a/Metadata/Texts Properties.xlsx
+++ b/Metadata/Texts Properties.xlsx
@@ -559,8 +559,10 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane xSplit="1.0" ySplit="1.0" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1" pane="topRight"/>
+      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
+      <selection activeCell="B2" sqref="B2" pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
@@ -644,7 +646,7 @@
         <v>13.0</v>
       </c>
       <c r="H2" s="2">
-        <v>97.0</v>
+        <v>31.0</v>
       </c>
       <c r="I2" s="2">
         <v>764.0</v>
@@ -663,7 +665,7 @@
       </c>
       <c r="M2" s="3">
         <f t="shared" ref="M2:M18" si="4">ROUND(H2/I2, 4)</f>
-        <v>0.127</v>
+        <v>0.0406</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>16</v>
@@ -692,7 +694,7 @@
         <v>6.0</v>
       </c>
       <c r="H3" s="2">
-        <v>98.0</v>
+        <v>28.0</v>
       </c>
       <c r="I3" s="2">
         <v>840.0</v>
@@ -711,7 +713,7 @@
       </c>
       <c r="M3" s="3">
         <f t="shared" si="4"/>
-        <v>0.1167</v>
+        <v>0.0333</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>18</v>
@@ -740,7 +742,7 @@
         <v>9.0</v>
       </c>
       <c r="H4" s="2">
-        <v>109.0</v>
+        <v>26.0</v>
       </c>
       <c r="I4" s="2">
         <v>767.0</v>
@@ -759,7 +761,7 @@
       </c>
       <c r="M4" s="3">
         <f t="shared" si="4"/>
-        <v>0.1421</v>
+        <v>0.0339</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>20</v>
@@ -788,7 +790,7 @@
         <v>8.0</v>
       </c>
       <c r="H5" s="2">
-        <v>87.0</v>
+        <v>30.0</v>
       </c>
       <c r="I5" s="2">
         <v>767.0</v>
@@ -807,7 +809,7 @@
       </c>
       <c r="M5" s="3">
         <f t="shared" si="4"/>
-        <v>0.1134</v>
+        <v>0.0391</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>22</v>
@@ -836,7 +838,7 @@
         <v>15.0</v>
       </c>
       <c r="H6" s="2">
-        <v>113.0</v>
+        <v>29.0</v>
       </c>
       <c r="I6" s="2">
         <v>764.0</v>
@@ -855,7 +857,7 @@
       </c>
       <c r="M6" s="3">
         <f t="shared" si="4"/>
-        <v>0.1479</v>
+        <v>0.038</v>
       </c>
       <c r="O6" s="4" t="s">
         <v>24</v>
@@ -884,7 +886,7 @@
         <v>11.0</v>
       </c>
       <c r="H7" s="2">
-        <v>96.0</v>
+        <v>26.0</v>
       </c>
       <c r="I7" s="2">
         <v>717.0</v>
@@ -903,7 +905,7 @@
       </c>
       <c r="M7" s="3">
         <f t="shared" si="4"/>
-        <v>0.1339</v>
+        <v>0.0363</v>
       </c>
       <c r="O7" s="4" t="s">
         <v>26</v>
@@ -932,7 +934,7 @@
         <v>13.0</v>
       </c>
       <c r="H8" s="2">
-        <v>116.0</v>
+        <v>33.0</v>
       </c>
       <c r="I8" s="2">
         <v>805.0</v>
@@ -951,7 +953,7 @@
       </c>
       <c r="M8" s="3">
         <f t="shared" si="4"/>
-        <v>0.1441</v>
+        <v>0.041</v>
       </c>
       <c r="O8" s="4" t="s">
         <v>28</v>
@@ -980,7 +982,7 @@
         <v>6.0</v>
       </c>
       <c r="H9" s="2">
-        <v>85.0</v>
+        <v>25.0</v>
       </c>
       <c r="I9" s="2">
         <v>782.0</v>
@@ -999,7 +1001,7 @@
       </c>
       <c r="M9" s="3">
         <f t="shared" si="4"/>
-        <v>0.1087</v>
+        <v>0.032</v>
       </c>
       <c r="O9" s="4" t="s">
         <v>30</v>
@@ -1028,7 +1030,7 @@
         <v>16.0</v>
       </c>
       <c r="H10" s="2">
-        <v>90.0</v>
+        <v>21.0</v>
       </c>
       <c r="I10" s="2">
         <v>708.0</v>
@@ -1047,7 +1049,7 @@
       </c>
       <c r="M10" s="3">
         <f t="shared" si="4"/>
-        <v>0.1271</v>
+        <v>0.0297</v>
       </c>
       <c r="O10" s="4" t="s">
         <v>32</v>
@@ -1076,7 +1078,7 @@
         <v>10.0</v>
       </c>
       <c r="H11" s="2">
-        <v>91.0</v>
+        <v>29.0</v>
       </c>
       <c r="I11" s="2">
         <v>742.0</v>
@@ -1095,7 +1097,7 @@
       </c>
       <c r="M11" s="3">
         <f t="shared" si="4"/>
-        <v>0.1226</v>
+        <v>0.0391</v>
       </c>
       <c r="O11" s="4" t="s">
         <v>34</v>
@@ -1124,7 +1126,7 @@
         <v>16.0</v>
       </c>
       <c r="H12" s="2">
-        <v>102.0</v>
+        <v>32.0</v>
       </c>
       <c r="I12" s="2">
         <v>714.0</v>
@@ -1143,7 +1145,7 @@
       </c>
       <c r="M12" s="3">
         <f t="shared" si="4"/>
-        <v>0.1429</v>
+        <v>0.0448</v>
       </c>
       <c r="O12" s="4" t="s">
         <v>36</v>
@@ -1172,7 +1174,7 @@
         <v>19.0</v>
       </c>
       <c r="H13" s="2">
-        <v>101.0</v>
+        <v>25.0</v>
       </c>
       <c r="I13" s="2">
         <v>707.0</v>
@@ -1191,7 +1193,7 @@
       </c>
       <c r="M13" s="3">
         <f t="shared" si="4"/>
-        <v>0.1429</v>
+        <v>0.0354</v>
       </c>
       <c r="O13" s="4" t="s">
         <v>38</v>
@@ -1220,7 +1222,7 @@
         <v>16.0</v>
       </c>
       <c r="H14" s="2">
-        <v>81.0</v>
+        <v>20.0</v>
       </c>
       <c r="I14" s="2">
         <v>706.0</v>
@@ -1239,7 +1241,7 @@
       </c>
       <c r="M14" s="3">
         <f t="shared" si="4"/>
-        <v>0.1147</v>
+        <v>0.0283</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>40</v>
@@ -1268,7 +1270,7 @@
         <v>10.0</v>
       </c>
       <c r="H15" s="2">
-        <v>125.0</v>
+        <v>38.0</v>
       </c>
       <c r="I15" s="2">
         <v>676.0</v>
@@ -1287,7 +1289,7 @@
       </c>
       <c r="M15" s="3">
         <f t="shared" si="4"/>
-        <v>0.1849</v>
+        <v>0.0562</v>
       </c>
       <c r="O15" s="4" t="s">
         <v>42</v>
@@ -1316,7 +1318,7 @@
         <v>24.0</v>
       </c>
       <c r="H16" s="2">
-        <v>167.0</v>
+        <v>64.0</v>
       </c>
       <c r="I16" s="2">
         <v>844.0</v>
@@ -1335,7 +1337,7 @@
       </c>
       <c r="M16" s="3">
         <f t="shared" si="4"/>
-        <v>0.1979</v>
+        <v>0.0758</v>
       </c>
       <c r="O16" s="4" t="s">
         <v>44</v>
@@ -1364,7 +1366,7 @@
         <v>11.0</v>
       </c>
       <c r="H17" s="2">
-        <v>118.0</v>
+        <v>41.0</v>
       </c>
       <c r="I17" s="2">
         <v>723.0</v>
@@ -1383,7 +1385,7 @@
       </c>
       <c r="M17" s="3">
         <f t="shared" si="4"/>
-        <v>0.1632</v>
+        <v>0.0567</v>
       </c>
       <c r="O17" s="4" t="s">
         <v>46</v>
@@ -1412,7 +1414,7 @@
         <v>17.0</v>
       </c>
       <c r="H18" s="2">
-        <v>140.0</v>
+        <v>75.0</v>
       </c>
       <c r="I18" s="2">
         <v>720.0</v>
@@ -1431,7 +1433,7 @@
       </c>
       <c r="M18" s="3">
         <f t="shared" si="4"/>
-        <v>0.1944</v>
+        <v>0.1042</v>
       </c>
       <c r="O18" s="2" t="s">
         <v>48</v>
@@ -1477,9 +1479,6 @@
       <c r="G20" s="2">
         <v>15.0</v>
       </c>
-      <c r="H20" s="2">
-        <v>158.0</v>
-      </c>
       <c r="I20" s="2">
         <v>1215.0</v>
       </c>
@@ -1495,10 +1494,7 @@
         <f t="shared" ref="L20:L22" si="7">ROUND(G20/I20, 4)</f>
         <v>0.0123</v>
       </c>
-      <c r="M20" s="3">
-        <f t="shared" ref="M20:M22" si="8">ROUND(H20/I20, 4)</f>
-        <v>0.13</v>
-      </c>
+      <c r="M20" s="3"/>
       <c r="N20" s="2" t="s">
         <v>51</v>
       </c>
@@ -1547,9 +1543,6 @@
       <c r="G21" s="2">
         <v>15.0</v>
       </c>
-      <c r="H21" s="2">
-        <v>99.0</v>
-      </c>
       <c r="I21" s="2">
         <v>752.0</v>
       </c>
@@ -1565,10 +1558,7 @@
         <f t="shared" si="7"/>
         <v>0.0199</v>
       </c>
-      <c r="M21" s="3">
-        <f t="shared" si="8"/>
-        <v>0.1316</v>
-      </c>
+      <c r="M21" s="3"/>
       <c r="O21" s="4" t="s">
         <v>54</v>
       </c>
@@ -1595,9 +1585,6 @@
       <c r="G22" s="2">
         <v>29.0</v>
       </c>
-      <c r="H22" s="2">
-        <v>273.0</v>
-      </c>
       <c r="I22" s="2">
         <v>1131.0</v>
       </c>
@@ -1613,10 +1600,7 @@
         <f t="shared" si="7"/>
         <v>0.0256</v>
       </c>
-      <c r="M22" s="3">
-        <f t="shared" si="8"/>
-        <v>0.2414</v>
-      </c>
+      <c r="M22" s="3"/>
       <c r="O22" s="4" t="s">
         <v>56</v>
       </c>
@@ -1656,15 +1640,15 @@
         <v>445.0</v>
       </c>
       <c r="J24" s="11">
-        <f t="shared" ref="J24:J26" si="9">ROUND(C24/E24, 4)</f>
+        <f t="shared" ref="J24:J26" si="8">ROUND(C24/E24, 4)</f>
         <v>0.08</v>
       </c>
       <c r="K24" s="11">
-        <f t="shared" ref="K24:K26" si="10">ROUND(D24/E24, 4)</f>
+        <f t="shared" ref="K24:K26" si="9">ROUND(D24/E24, 4)</f>
         <v>0.2</v>
       </c>
       <c r="L24" s="11">
-        <f t="shared" ref="L24:L26" si="11">ROUND(G24/I24, 4)</f>
+        <f t="shared" ref="L24:L26" si="10">ROUND(G24/I24, 4)</f>
         <v>0.018</v>
       </c>
       <c r="M24" s="3"/>
@@ -1719,15 +1703,15 @@
         <v>825.0</v>
       </c>
       <c r="J25" s="14">
+        <f t="shared" si="8"/>
+        <v>0.378</v>
+      </c>
+      <c r="K25" s="11">
         <f t="shared" si="9"/>
-        <v>0.378</v>
-      </c>
-      <c r="K25" s="11">
+        <v>0.0488</v>
+      </c>
+      <c r="L25" s="14">
         <f t="shared" si="10"/>
-        <v>0.0488</v>
-      </c>
-      <c r="L25" s="14">
-        <f t="shared" si="11"/>
         <v>0.0388</v>
       </c>
       <c r="M25" s="3"/>
@@ -1782,15 +1766,15 @@
         <v>787.0</v>
       </c>
       <c r="J26" s="11">
+        <f t="shared" si="8"/>
+        <v>0.1333</v>
+      </c>
+      <c r="K26" s="14">
         <f t="shared" si="9"/>
-        <v>0.1333</v>
-      </c>
-      <c r="K26" s="14">
+        <v>0.4333</v>
+      </c>
+      <c r="L26" s="11">
         <f t="shared" si="10"/>
-        <v>0.4333</v>
-      </c>
-      <c r="L26" s="11">
-        <f t="shared" si="11"/>
         <v>0.0102</v>
       </c>
       <c r="M26" s="3"/>

</xml_diff>